<commit_message>
Update English technical paper
</commit_message>
<xml_diff>
--- a/gf-bench/results/results-2022-05-24.xlsx
+++ b/gf-bench/results/results-2022-05-24.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="21">
   <si>
     <t xml:space="preserve">Multiplication</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t xml:space="preserve">gf-nishida-region-16-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speed (MB/s)</t>
   </si>
 </sst>
 </file>
@@ -227,15 +224,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -311,10 +299,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.341697997726677"/>
-          <c:y val="0.0194897236002835"/>
-          <c:w val="0.586954620967037"/>
-          <c:h val="0.814759036144578"/>
+          <c:x val="0.341704585229261"/>
+          <c:y val="0.0194914503411004"/>
+          <c:w val="0.58689184459223"/>
+          <c:h val="0.814654026756445"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -493,11 +481,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="55167030"/>
-        <c:axId val="64687722"/>
+        <c:axId val="57631062"/>
+        <c:axId val="25911997"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55167030"/>
+        <c:axId val="57631062"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -525,7 +513,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64687722"/>
+        <c:crossAx val="25911997"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -533,7 +521,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64687722"/>
+        <c:axId val="25911997"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -572,8 +560,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.373611961178631"/>
-              <c:y val="0.894578313253012"/>
+              <c:x val="0.37355617780889"/>
+              <c:y val="0.894480375653406"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -606,7 +594,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55167030"/>
+        <c:crossAx val="57631062"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -792,11 +780,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="5650651"/>
-        <c:axId val="9413280"/>
+        <c:axId val="42869493"/>
+        <c:axId val="19611600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5650651"/>
+        <c:axId val="42869493"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -824,7 +812,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9413280"/>
+        <c:crossAx val="19611600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -832,7 +820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9413280"/>
+        <c:axId val="19611600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -871,8 +859,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.404212550253452"/>
-              <c:y val="0.879840362420451"/>
+              <c:x val="0.404251596535736"/>
+              <c:y val="0.879719525350593"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -905,7 +893,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5650651"/>
+        <c:crossAx val="42869493"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -944,10 +932,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.34161056221037"/>
-          <c:y val="0.0194897236002835"/>
-          <c:w val="0.586954620967037"/>
-          <c:h val="0.81467044649185"/>
+          <c:x val="0.341617080854043"/>
+          <c:y val="0.0194914503411004"/>
+          <c:w val="0.58689184459223"/>
+          <c:h val="0.814565429254895"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1120,11 +1108,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="903055"/>
-        <c:axId val="90458165"/>
+        <c:axId val="39263881"/>
+        <c:axId val="17701830"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="903055"/>
+        <c:axId val="39263881"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1152,7 +1140,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90458165"/>
+        <c:crossAx val="17701830"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1160,7 +1148,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90458165"/>
+        <c:axId val="17701830"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,8 +1187,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.373611961178631"/>
-              <c:y val="0.894578313253012"/>
+              <c:x val="0.37355617780889"/>
+              <c:y val="0.894480375653406"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1233,7 +1221,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="903055"/>
+        <c:crossAx val="39263881"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1419,11 +1407,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="74046385"/>
-        <c:axId val="41646596"/>
+        <c:axId val="82542932"/>
+        <c:axId val="34946488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74046385"/>
+        <c:axId val="82542932"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,7 +1439,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41646596"/>
+        <c:crossAx val="34946488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1459,7 +1447,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41646596"/>
+        <c:axId val="34946488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1498,8 +1486,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.404422690324272"/>
-              <c:y val="0.879840362420451"/>
+              <c:x val="0.404478656403079"/>
+              <c:y val="0.879719525350593"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1532,7 +1520,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74046385"/>
+        <c:crossAx val="82542932"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1570,9 +1558,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>650160</xdr:colOff>
+      <xdr:colOff>649800</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1580,8 +1568,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7775280" y="0"/>
-        <a:ext cx="4116960" cy="4063320"/>
+        <a:off x="7773120" y="0"/>
+        <a:ext cx="4113720" cy="4062960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1600,9 +1588,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>344160</xdr:colOff>
+      <xdr:colOff>343800</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1610,8 +1598,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15095160" y="210240"/>
-        <a:ext cx="4118760" cy="3337200"/>
+        <a:off x="15089040" y="210240"/>
+        <a:ext cx="4114800" cy="3336840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1635,9 +1623,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>539280</xdr:colOff>
+      <xdr:colOff>538920</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1645,8 +1633,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7664400" y="0"/>
-        <a:ext cx="4116960" cy="4063320"/>
+        <a:off x="7662240" y="0"/>
+        <a:ext cx="4113720" cy="4062960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1665,9 +1653,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>369720</xdr:colOff>
+      <xdr:colOff>369360</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1675,8 +1663,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15321600" y="360"/>
-        <a:ext cx="4118400" cy="3337200"/>
+        <a:off x="15314400" y="360"/>
+        <a:ext cx="4115160" cy="3336840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1700,7 +1688,7 @@
       <selection pane="topLeft" activeCell="V33" activeCellId="0" sqref="V33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.71"/>
@@ -2156,11 +2144,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.71"/>
@@ -2586,204 +2574,129 @@
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="H24" s="0" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="G25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="5" t="n">
-        <v>3209.972985</v>
-      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="G26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="5" t="n">
-        <v>1708.165867</v>
-      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="G27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H27" s="5" t="n">
-        <v>1075.702116</v>
-      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="G28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="5" t="n">
-        <v>816.556187</v>
-      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="G29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H29" s="5" t="n">
-        <v>656.68379</v>
-      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
-      <c r="G30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="5" t="n">
-        <v>330.859085</v>
-      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
-      <c r="G31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="5" t="n">
-        <v>196.973926</v>
-      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
-      <c r="G32" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H32" s="5" t="n">
-        <v>196.843393</v>
-      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
-      <c r="G33" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H33" s="5" t="n">
-        <v>69.921408</v>
-      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="G34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="5" t="n">
-        <v>67.242343</v>
-      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="G35" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="5" t="n">
-        <v>63.007019</v>
-      </c>
+      <c r="G35" s="4"/>
+      <c r="H35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
-      <c r="G36" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="5" t="n">
-        <v>45.991832</v>
-      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="G37" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H37" s="5" t="n">
-        <v>40.576659</v>
-      </c>
+      <c r="G37" s="4"/>
+      <c r="H37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
-      <c r="G38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="5" t="n">
-        <v>40.316124</v>
-      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
-      <c r="G39" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H39" s="5" t="n">
-        <v>39.223663</v>
-      </c>
+      <c r="G39" s="4"/>
+      <c r="H39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
-      <c r="G40" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40" s="5" t="n">
-        <v>34.786186</v>
-      </c>
+      <c r="G40" s="4"/>
+      <c r="H40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
-      <c r="G41" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" s="5" t="n">
-        <v>26.800339</v>
-      </c>
+      <c r="G41" s="4"/>
+      <c r="H41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G42" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H42" s="5" t="n">
-        <v>2.780645</v>
-      </c>
+      <c r="G42" s="4"/>
+      <c r="H42" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>